<commit_message>
atualizacao de github page e de bases de dados para 2a RQ do PLAN2-29"
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2024/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2024/crescimento_mercado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Geracao Distribuida\PDE\PLAN25-29\dados_premissas\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Geracao Distribuida\PDE\PLAN25-29_2RQ\dados_premissas\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2E372A-62F9-4F66-A830-7FE49F247B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD57A059-69CE-451B-8F38-760E74E808D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2445" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -379,12 +379,12 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -527,7 +527,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>2.1999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4"/>
@@ -537,7 +537,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>2.3E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>

</xml_diff>

<commit_message>
atualizacao dados PLAN 2026-30
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2024/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2024/crescimento_mercado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Geracao Distribuida\PDE\PLAN25-29_2RQ\dados_premissas\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Geracao Distribuida\PDE\PLAN26-30\dados_premissas\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD57A059-69CE-451B-8F38-760E74E808D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB39BD6A-0B10-480F-A105-CAA245680FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="615" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -378,13 +378,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -537,7 +537,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
@@ -547,7 +547,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>2.5000000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
@@ -557,7 +557,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
@@ -567,7 +567,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
@@ -577,7 +577,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
@@ -587,7 +587,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
@@ -597,7 +597,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
@@ -607,7 +607,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
@@ -617,7 +617,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
@@ -627,7 +627,7 @@
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
@@ -637,7 +637,7 @@
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
@@ -647,7 +647,7 @@
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
@@ -657,7 +657,7 @@
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
@@ -667,7 +667,7 @@
         <v>2039</v>
       </c>
       <c r="B31">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
@@ -677,7 +677,7 @@
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
@@ -687,7 +687,7 @@
         <v>2041</v>
       </c>
       <c r="B33">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>2042</v>
       </c>
       <c r="B34">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -703,7 +703,7 @@
         <v>2043</v>
       </c>
       <c r="B35">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -711,7 +711,7 @@
         <v>2044</v>
       </c>
       <c r="B36">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -719,7 +719,7 @@
         <v>2045</v>
       </c>
       <c r="B37">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>2046</v>
       </c>
       <c r="B38">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>2047</v>
       </c>
       <c r="B39">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -743,7 +743,7 @@
         <v>2048</v>
       </c>
       <c r="B40">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>2049</v>
       </c>
       <c r="B41">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -759,7 +759,7 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -767,7 +767,7 @@
         <v>2051</v>
       </c>
       <c r="B43">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -775,7 +775,7 @@
         <v>2052</v>
       </c>
       <c r="B44">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>2053</v>
       </c>
       <c r="B45">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -791,7 +791,7 @@
         <v>2054</v>
       </c>
       <c r="B46">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -799,7 +799,7 @@
         <v>2055</v>
       </c>
       <c r="B47">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>2056</v>
       </c>
       <c r="B48">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -815,7 +815,7 @@
         <v>2057</v>
       </c>
       <c r="B49">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -823,7 +823,7 @@
         <v>2058</v>
       </c>
       <c r="B50">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
         <v>2059</v>
       </c>
       <c r="B51">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -839,7 +839,7 @@
         <v>2060</v>
       </c>
       <c r="B52">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>